<commit_message>
updated voltage divider calculations
</commit_message>
<xml_diff>
--- a/references/voltageDividerCalculations.xlsx
+++ b/references/voltageDividerCalculations.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19530" windowHeight="10650"/>
   </bookViews>
   <sheets>
-    <sheet name="Dividers" sheetId="1" r:id="rId1"/>
-    <sheet name="Resistors" sheetId="2" r:id="rId2"/>
+    <sheet name="Dividers" sheetId="3" r:id="rId1"/>
+    <sheet name="100kDividers" sheetId="1" r:id="rId2"/>
+    <sheet name="Resistors" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Level ID</t>
   </si>
@@ -110,13 +111,28 @@
   <si>
     <t>ERJ-8ENF6202V</t>
   </si>
+  <si>
+    <t>Levels</t>
+  </si>
+  <si>
+    <t>http://www.electronics2000.co.uk/calc/potential-divider-calculator.php</t>
+  </si>
+  <si>
+    <t>Typ</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>use these:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -163,13 +179,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,9 +469,2051 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE23" sqref="AE23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3.3</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0.01</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E19" si="0">C2/D2</f>
+        <v>6.2500000000000001E-4</v>
+      </c>
+      <c r="F2">
+        <f>E2*A2</f>
+        <v>2.0625000000000001E-3</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>0.1</v>
+      </c>
+      <c r="I2">
+        <f>(H2*0.95)/(G2*1.05+H2*0.95)</f>
+        <v>9.0394405062086682E-4</v>
+      </c>
+      <c r="J2">
+        <f>H2/(G2+H2)</f>
+        <v>9.9900099900099922E-4</v>
+      </c>
+      <c r="K2">
+        <f>(H2*1.05)/(G2*0.95+H2*1.05)</f>
+        <v>1.1040428999526839E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3.3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F19" si="1">E3*A3</f>
+        <v>0.10312499999999999</v>
+      </c>
+      <c r="G3" s="6">
+        <v>100</v>
+      </c>
+      <c r="H3" s="6">
+        <v>3.3</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I19" si="2">(H3*0.95)/(G3*1.05+H3*0.95)</f>
+        <v>2.8991538354834232E-2</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J19" si="3">H3/(G3+H3)</f>
+        <v>3.1945788964181994E-2</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K19" si="4">(H3*1.05)/(G3*0.95+H3*1.05)</f>
+        <v>3.5190169095617729E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3.3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f>C3+1</f>
+        <v>1.5</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>9.375E-2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0.30937499999999996</v>
+      </c>
+      <c r="G4" s="7">
+        <v>82</v>
+      </c>
+      <c r="H4" s="7">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>9.9372384937238489E-2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>0.10869565217391304</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="4"/>
+        <v>0.11877828054298643</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3.3</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C18" si="5">C4+1</f>
+        <v>2.5</v>
+      </c>
+      <c r="D5">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.15625</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.515625</v>
+      </c>
+      <c r="G5" s="6">
+        <v>82</v>
+      </c>
+      <c r="H5" s="6">
+        <v>15</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>0.1420029895366218</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>0.15463917525773196</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="4"/>
+        <v>0.16817939135077417</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3.3</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="5"/>
+        <v>3.5</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.21875</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.72187499999999993</v>
+      </c>
+      <c r="G6" s="7">
+        <v>82</v>
+      </c>
+      <c r="H6" s="7">
+        <v>22</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>0.1953271028037383</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>0.21153846153846154</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>0.22871287128712872</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3.3</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="5"/>
+        <v>4.5</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.28125</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.92812499999999998</v>
+      </c>
+      <c r="G7" s="6">
+        <v>68</v>
+      </c>
+      <c r="H7" s="6">
+        <v>27</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>0.26429675425038635</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>0.28421052631578947</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>0.30500268961807431</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3.3</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="5"/>
+        <v>5.5</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.34375</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1.1343749999999999</v>
+      </c>
+      <c r="G8" s="7">
+        <v>68</v>
+      </c>
+      <c r="H8" s="7">
+        <v>33</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>0.30510948905109486</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>0.32673267326732675</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="4"/>
+        <v>0.34911838790931987</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3.3</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="5"/>
+        <v>6.5</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.40625</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1.340625</v>
+      </c>
+      <c r="G9" s="6">
+        <v>56</v>
+      </c>
+      <c r="H9" s="6">
+        <v>39</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>0.38654147104851327</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>0.41052631578947368</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>0.43494423791821563</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3.3</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="5"/>
+        <v>7.5</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.46875</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>1.546875</v>
+      </c>
+      <c r="G10" s="7">
+        <v>56</v>
+      </c>
+      <c r="H10" s="7">
+        <v>47</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>0.43160947317544707</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>0.4563106796116505</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>0.48122866894197958</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3.3</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="5"/>
+        <v>8.5</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.53125</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>1.7531249999999998</v>
+      </c>
+      <c r="G11">
+        <v>47</v>
+      </c>
+      <c r="H11">
+        <v>56</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>0.51877133105802042</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>0.5436893203883495</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>0.56839052682455293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3.3</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="5"/>
+        <v>9.5</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.59375</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>1.9593749999999999</v>
+      </c>
+      <c r="G12" s="6">
+        <v>39</v>
+      </c>
+      <c r="H12" s="6">
+        <v>56</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>0.56505576208178432</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>0.58947368421052626</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>0.61345852895148678</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3.3</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="5"/>
+        <v>10.5</v>
+      </c>
+      <c r="D13">
+        <v>16</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.65625</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>2.1656249999999999</v>
+      </c>
+      <c r="G13" s="7">
+        <v>33</v>
+      </c>
+      <c r="H13" s="7">
+        <v>68</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>0.65088161209068007</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>0.67326732673267331</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>0.69489051094890519</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3.3</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="5"/>
+        <v>11.5</v>
+      </c>
+      <c r="D14">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.71875</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>2.3718749999999997</v>
+      </c>
+      <c r="G14" s="6">
+        <v>27</v>
+      </c>
+      <c r="H14" s="6">
+        <v>68</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>0.6949973103819258</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>0.71578947368421053</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>0.73570324574961354</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3.3</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="5"/>
+        <v>12.5</v>
+      </c>
+      <c r="D15">
+        <v>16</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.78125</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>2.578125</v>
+      </c>
+      <c r="G15" s="7">
+        <v>22</v>
+      </c>
+      <c r="H15" s="7">
+        <v>82</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>0.7712871287128712</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>0.78846153846153844</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>0.80467289719626178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3.3</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="5"/>
+        <v>13.5</v>
+      </c>
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.84375</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>2.7843749999999998</v>
+      </c>
+      <c r="G16" s="6">
+        <v>15</v>
+      </c>
+      <c r="H16" s="6">
+        <v>82</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>0.8318206086492258</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>0.84536082474226804</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>0.85799701046337817</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3.3</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="5"/>
+        <v>14.5</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.90625</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>2.9906249999999996</v>
+      </c>
+      <c r="G17" s="7">
+        <v>10</v>
+      </c>
+      <c r="H17" s="7">
+        <v>82</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>0.88122171945701355</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>0.89130434782608692</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>0.90062761506276157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3.3</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="5"/>
+        <v>15.5</v>
+      </c>
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0.96875</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>3.1968749999999999</v>
+      </c>
+      <c r="G18" s="6">
+        <v>3.3</v>
+      </c>
+      <c r="H18" s="6">
+        <v>100</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>0.96480983090438222</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>0.96805421103581801</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>0.97100846164516574</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3.3</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>15.99</v>
+      </c>
+      <c r="D19">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0.99937500000000001</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>3.2979374999999997</v>
+      </c>
+      <c r="G19">
+        <v>0.01</v>
+      </c>
+      <c r="H19">
+        <v>100</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>0.99988948589892701</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>0.99990000999900008</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>0.99990953199472421</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3.3</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0.01</v>
+      </c>
+      <c r="D27">
+        <v>23</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ref="E27:E43" si="6">C27/D27</f>
+        <v>4.3478260869565219E-4</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F27:F43" si="7">E27*A27</f>
+        <v>1.4347826086956522E-3</v>
+      </c>
+      <c r="G27" s="6">
+        <v>100</v>
+      </c>
+      <c r="H27" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ref="I27" si="8">(H27*0.95)/(G27*1.05+H27*0.95)</f>
+        <v>9.0394405062086682E-4</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ref="J27" si="9">H27/(G27+H27)</f>
+        <v>9.9900099900099922E-4</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ref="K27" si="10">(H27*1.05)/(G27*0.95+H27*1.05)</f>
+        <v>1.1040428999526839E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3.3</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="D28">
+        <v>23</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="6"/>
+        <v>2.1739130434782608E-2</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="7"/>
+        <v>7.1739130434782597E-2</v>
+      </c>
+      <c r="G28" s="7">
+        <v>100</v>
+      </c>
+      <c r="H28" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I28">
+        <f t="shared" ref="I28:I51" si="11">(H28*0.95)/(G28*1.05+H28*0.95)</f>
+        <v>1.9516294705387991E-2</v>
+      </c>
+      <c r="J28">
+        <f t="shared" ref="J28:J51" si="12">H28/(G28+H28)</f>
+        <v>2.1526418786692762E-2</v>
+      </c>
+      <c r="K28">
+        <f t="shared" ref="K28:K51" si="13">(H28*1.05)/(G28*0.95+H28*1.05)</f>
+        <v>2.3738567464803212E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3.3</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f>C28+1</f>
+        <v>1.5</v>
+      </c>
+      <c r="D29">
+        <v>23</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="6"/>
+        <v>6.5217391304347824E-2</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="7"/>
+        <v>0.2152173913043478</v>
+      </c>
+      <c r="G29" s="7">
+        <v>100</v>
+      </c>
+      <c r="H29" s="7">
+        <v>6.8</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="11"/>
+        <v>5.7958011842813566E-2</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="12"/>
+        <v>6.3670411985018729E-2</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="13"/>
+        <v>6.9904053260231053E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3.3</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:C50" si="14">C29+1</f>
+        <v>2.5</v>
+      </c>
+      <c r="D30">
+        <v>23</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="6"/>
+        <v>0.10869565217391304</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="7"/>
+        <v>0.35869565217391303</v>
+      </c>
+      <c r="G30" s="7">
+        <v>82</v>
+      </c>
+      <c r="H30" s="7">
+        <v>10</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="11"/>
+        <v>9.9372384937238489E-2</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="12"/>
+        <v>0.10869565217391304</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="13"/>
+        <v>0.11877828054298643</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3.3</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="14"/>
+        <v>3.5</v>
+      </c>
+      <c r="D31">
+        <v>23</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="6"/>
+        <v>0.15217391304347827</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="7"/>
+        <v>0.50217391304347825</v>
+      </c>
+      <c r="G31" s="6">
+        <v>82</v>
+      </c>
+      <c r="H31" s="6">
+        <v>15</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="11"/>
+        <v>0.1420029895366218</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="12"/>
+        <v>0.15463917525773196</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="13"/>
+        <v>0.16817939135077417</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3.3</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="14"/>
+        <v>4.5</v>
+      </c>
+      <c r="D32">
+        <v>23</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="6"/>
+        <v>0.19565217391304349</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="7"/>
+        <v>0.64565217391304353</v>
+      </c>
+      <c r="G32" s="7">
+        <v>82</v>
+      </c>
+      <c r="H32" s="7">
+        <v>18</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="11"/>
+        <v>0.16569767441860461</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="12"/>
+        <v>0.18</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="13"/>
+        <v>0.19524793388429754</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3.3</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="14"/>
+        <v>5.5</v>
+      </c>
+      <c r="D33">
+        <v>23</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="6"/>
+        <v>0.2391304347826087</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="7"/>
+        <v>0.78913043478260869</v>
+      </c>
+      <c r="G33" s="7">
+        <v>82</v>
+      </c>
+      <c r="H33" s="7">
+        <v>22</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="11"/>
+        <v>0.1953271028037383</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="12"/>
+        <v>0.21153846153846154</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="13"/>
+        <v>0.22871287128712872</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3.3</v>
+      </c>
+      <c r="B34">
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="14"/>
+        <v>6.5</v>
+      </c>
+      <c r="D34">
+        <v>23</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="6"/>
+        <v>0.28260869565217389</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="7"/>
+        <v>0.93260869565217375</v>
+      </c>
+      <c r="G34" s="7">
+        <v>68</v>
+      </c>
+      <c r="H34" s="7">
+        <v>27</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="11"/>
+        <v>0.26429675425038635</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="12"/>
+        <v>0.28421052631578947</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="13"/>
+        <v>0.30500268961807431</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3.3</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="14"/>
+        <v>7.5</v>
+      </c>
+      <c r="D35">
+        <v>23</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="6"/>
+        <v>0.32608695652173914</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="7"/>
+        <v>1.076086956521739</v>
+      </c>
+      <c r="G35" s="6">
+        <v>68</v>
+      </c>
+      <c r="H35" s="6">
+        <v>33</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="11"/>
+        <v>0.30510948905109486</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="12"/>
+        <v>0.32673267326732675</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="13"/>
+        <v>0.34911838790931987</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>3.3</v>
+      </c>
+      <c r="B36">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="14"/>
+        <v>8.5</v>
+      </c>
+      <c r="D36">
+        <v>23</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="6"/>
+        <v>0.36956521739130432</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="7"/>
+        <v>1.2195652173913043</v>
+      </c>
+      <c r="G36">
+        <v>68</v>
+      </c>
+      <c r="H36">
+        <v>39</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="11"/>
+        <v>0.34163208852005528</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="12"/>
+        <v>0.3644859813084112</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="13"/>
+        <v>0.38796778777830415</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3.3</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="14"/>
+        <v>9.5</v>
+      </c>
+      <c r="D37">
+        <v>23</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="6"/>
+        <v>0.41304347826086957</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="7"/>
+        <v>1.3630434782608696</v>
+      </c>
+      <c r="G37" s="7">
+        <v>56</v>
+      </c>
+      <c r="H37" s="7">
+        <v>39</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="11"/>
+        <v>0.38654147104851327</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="12"/>
+        <v>0.41052631578947368</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="13"/>
+        <v>0.43494423791821563</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3.3</v>
+      </c>
+      <c r="B38">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="14"/>
+        <v>10.5</v>
+      </c>
+      <c r="D38">
+        <v>23</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="6"/>
+        <v>0.45652173913043476</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="7"/>
+        <v>1.5065217391304346</v>
+      </c>
+      <c r="G38" s="7">
+        <v>56</v>
+      </c>
+      <c r="H38" s="7">
+        <v>47</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="11"/>
+        <v>0.43160947317544707</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="12"/>
+        <v>0.4563106796116505</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="13"/>
+        <v>0.48122866894197958</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3.3</v>
+      </c>
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="14"/>
+        <v>11.5</v>
+      </c>
+      <c r="D39">
+        <v>23</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="7"/>
+        <v>1.65</v>
+      </c>
+      <c r="G39" s="6">
+        <v>47</v>
+      </c>
+      <c r="H39" s="6">
+        <v>47</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="11"/>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="13"/>
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3.3</v>
+      </c>
+      <c r="B40">
+        <v>13</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="14"/>
+        <v>12.5</v>
+      </c>
+      <c r="D40">
+        <v>23</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="6"/>
+        <v>0.54347826086956519</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="7"/>
+        <v>1.793478260869565</v>
+      </c>
+      <c r="G40" s="7">
+        <v>47</v>
+      </c>
+      <c r="H40" s="7">
+        <v>56</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="11"/>
+        <v>0.51877133105802042</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="12"/>
+        <v>0.5436893203883495</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="13"/>
+        <v>0.56839052682455293</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>3.3</v>
+      </c>
+      <c r="B41">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="14"/>
+        <v>13.5</v>
+      </c>
+      <c r="D41">
+        <v>23</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="6"/>
+        <v>0.58695652173913049</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="7"/>
+        <v>1.9369565217391305</v>
+      </c>
+      <c r="G41" s="7">
+        <v>39</v>
+      </c>
+      <c r="H41" s="7">
+        <v>56</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="11"/>
+        <v>0.56505576208178432</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="12"/>
+        <v>0.58947368421052626</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="13"/>
+        <v>0.61345852895148678</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>3.3</v>
+      </c>
+      <c r="B42">
+        <v>15</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="14"/>
+        <v>14.5</v>
+      </c>
+      <c r="D42">
+        <v>23</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="6"/>
+        <v>0.63043478260869568</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="7"/>
+        <v>2.0804347826086955</v>
+      </c>
+      <c r="G42" s="7">
+        <v>39</v>
+      </c>
+      <c r="H42" s="7">
+        <v>68</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="11"/>
+        <v>0.61203221222169579</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="12"/>
+        <v>0.63551401869158874</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="13"/>
+        <v>0.65836791147994467</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>3.3</v>
+      </c>
+      <c r="B43">
+        <v>16</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="14"/>
+        <v>15.5</v>
+      </c>
+      <c r="D43">
+        <v>23</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="6"/>
+        <v>0.67391304347826086</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="7"/>
+        <v>2.2239130434782606</v>
+      </c>
+      <c r="G43" s="6">
+        <v>33</v>
+      </c>
+      <c r="H43" s="6">
+        <v>68</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="11"/>
+        <v>0.65088161209068007</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="12"/>
+        <v>0.67326732673267331</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="13"/>
+        <v>0.69489051094890519</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>3.3</v>
+      </c>
+      <c r="B44">
+        <v>17</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="14"/>
+        <v>16.5</v>
+      </c>
+      <c r="D44">
+        <v>23</v>
+      </c>
+      <c r="E44">
+        <f t="shared" ref="E44:E51" si="15">C44/D44</f>
+        <v>0.71739130434782605</v>
+      </c>
+      <c r="F44">
+        <f t="shared" ref="F44:F51" si="16">E44*A44</f>
+        <v>2.3673913043478256</v>
+      </c>
+      <c r="G44" s="7">
+        <v>27</v>
+      </c>
+      <c r="H44" s="7">
+        <v>68</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="11"/>
+        <v>0.6949973103819258</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="12"/>
+        <v>0.71578947368421053</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="13"/>
+        <v>0.73570324574961354</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>3.3</v>
+      </c>
+      <c r="B45">
+        <v>18</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="14"/>
+        <v>17.5</v>
+      </c>
+      <c r="D45">
+        <v>23</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="15"/>
+        <v>0.76086956521739135</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="16"/>
+        <v>2.5108695652173911</v>
+      </c>
+      <c r="G45" s="7">
+        <v>22</v>
+      </c>
+      <c r="H45" s="7">
+        <v>82</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="11"/>
+        <v>0.7712871287128712</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="12"/>
+        <v>0.78846153846153844</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="13"/>
+        <v>0.80467289719626178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>3.3</v>
+      </c>
+      <c r="B46">
+        <v>19</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="14"/>
+        <v>18.5</v>
+      </c>
+      <c r="D46">
+        <v>23</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="15"/>
+        <v>0.80434782608695654</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="16"/>
+        <v>2.6543478260869566</v>
+      </c>
+      <c r="G46" s="7">
+        <v>18</v>
+      </c>
+      <c r="H46" s="7">
+        <v>82</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="11"/>
+        <v>0.80475206611570238</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="12"/>
+        <v>0.82</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="13"/>
+        <v>0.83430232558139539</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3.3</v>
+      </c>
+      <c r="B47">
+        <v>20</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="14"/>
+        <v>19.5</v>
+      </c>
+      <c r="D47">
+        <v>23</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="15"/>
+        <v>0.84782608695652173</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="16"/>
+        <v>2.7978260869565217</v>
+      </c>
+      <c r="G47" s="6">
+        <v>15</v>
+      </c>
+      <c r="H47" s="6">
+        <v>82</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="11"/>
+        <v>0.8318206086492258</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="12"/>
+        <v>0.84536082474226804</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="13"/>
+        <v>0.85799701046337817</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>3.3</v>
+      </c>
+      <c r="B48">
+        <v>21</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="14"/>
+        <v>20.5</v>
+      </c>
+      <c r="D48">
+        <v>23</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="15"/>
+        <v>0.89130434782608692</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="16"/>
+        <v>2.9413043478260867</v>
+      </c>
+      <c r="G48" s="7">
+        <v>10</v>
+      </c>
+      <c r="H48" s="7">
+        <v>82</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="11"/>
+        <v>0.88122171945701355</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="12"/>
+        <v>0.89130434782608692</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="13"/>
+        <v>0.90062761506276157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3.3</v>
+      </c>
+      <c r="B49">
+        <v>22</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="14"/>
+        <v>21.5</v>
+      </c>
+      <c r="D49">
+        <v>23</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="15"/>
+        <v>0.93478260869565222</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="16"/>
+        <v>3.0847826086956522</v>
+      </c>
+      <c r="G49" s="7">
+        <v>6.8</v>
+      </c>
+      <c r="H49" s="7">
+        <v>100</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="11"/>
+        <v>0.93009594673976892</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="12"/>
+        <v>0.93632958801498134</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="13"/>
+        <v>0.94204198815718654</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3.3</v>
+      </c>
+      <c r="B50">
+        <v>23</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="14"/>
+        <v>22.5</v>
+      </c>
+      <c r="D50">
+        <v>23</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="15"/>
+        <v>0.97826086956521741</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="16"/>
+        <v>3.2282608695652173</v>
+      </c>
+      <c r="G50" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H50" s="7">
+        <v>100</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="11"/>
+        <v>0.97626143253519682</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="12"/>
+        <v>0.97847358121330719</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="13"/>
+        <v>0.98048370529461193</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>3.3</v>
+      </c>
+      <c r="B51">
+        <v>24</v>
+      </c>
+      <c r="C51">
+        <v>22.99</v>
+      </c>
+      <c r="D51">
+        <v>23</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="15"/>
+        <v>0.99956521739130433</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="16"/>
+        <v>3.298565217391304</v>
+      </c>
+      <c r="G51" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H51" s="6">
+        <v>100</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="11"/>
+        <v>0.9988959571000473</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="12"/>
+        <v>0.99900099900099903</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="13"/>
+        <v>0.99909605594937911</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F55" s="7">
+        <v>100</v>
+      </c>
+      <c r="G55" s="7">
+        <f>COUNTIF($G$27:$H$51,F55)</f>
+        <v>6</v>
+      </c>
+      <c r="H55" s="7">
+        <v>2</v>
+      </c>
+      <c r="I55" s="7">
+        <f>G55+H55</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F56" s="7">
+        <v>82</v>
+      </c>
+      <c r="G56" s="7">
+        <f t="shared" ref="G56:G69" si="17">COUNTIF($G$27:$H$51,F56)</f>
+        <v>8</v>
+      </c>
+      <c r="H56" s="7">
+        <v>2</v>
+      </c>
+      <c r="I56" s="7">
+        <f t="shared" ref="I56:I69" si="18">G56+H56</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F57" s="7">
+        <v>68</v>
+      </c>
+      <c r="G57" s="7">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="I57" s="7">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F58" s="7">
+        <v>56</v>
+      </c>
+      <c r="G58" s="7">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="H58" s="7">
+        <v>2</v>
+      </c>
+      <c r="I58" s="7">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F59" s="7">
+        <v>47</v>
+      </c>
+      <c r="G59" s="7">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="I59" s="7">
+        <f t="shared" si="18"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F60" s="7">
+        <v>39</v>
+      </c>
+      <c r="G60" s="7">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="H60" s="7">
+        <v>2</v>
+      </c>
+      <c r="I60" s="7">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F61" s="7">
+        <v>33</v>
+      </c>
+      <c r="G61" s="7">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="I61" s="7">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F62" s="7">
+        <v>27</v>
+      </c>
+      <c r="G62" s="7">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="I62" s="7">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F63" s="7">
+        <v>22</v>
+      </c>
+      <c r="G63" s="7">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="I63" s="7">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F64" s="7">
+        <v>18</v>
+      </c>
+      <c r="G64" s="7">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="H64" s="7">
+        <v>2</v>
+      </c>
+      <c r="I64" s="7">
+        <f t="shared" si="18"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F65" s="7">
+        <v>15</v>
+      </c>
+      <c r="G65" s="7">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="I65" s="7">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F66" s="7">
+        <v>10</v>
+      </c>
+      <c r="G66" s="7">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="I66" s="7">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F67" s="7">
+        <v>6.8</v>
+      </c>
+      <c r="G67" s="7">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="I67" s="7">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F68" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G68" s="7">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="I68" s="7">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G69" s="7">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="I69" s="7">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="6:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P22" workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="Y38" sqref="Y38"/>
     </sheetView>
   </sheetViews>
@@ -561,7 +2621,7 @@
         <v>33000</v>
       </c>
       <c r="J2" s="2">
-        <f>I2*A2/E2-I2</f>
+        <f t="shared" ref="J2:J19" si="1">I2*A2/E2-I2</f>
         <v>52767000</v>
       </c>
       <c r="K2" s="3">
@@ -573,7 +2633,7 @@
         <v>527.66999999999996</v>
       </c>
       <c r="N2">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L2)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L2),,)),,),0))</f>
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L2)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L2),,)),,),0))</f>
         <v>560</v>
       </c>
       <c r="O2">
@@ -585,7 +2645,7 @@
         <v>5.7732142857142857E-2</v>
       </c>
       <c r="R2">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L2)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L2),,)),,),0))</f>
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L2)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L2),,)),,),0))</f>
         <v>510</v>
       </c>
       <c r="S2">
@@ -597,7 +2657,7 @@
         <v>3.4647058823529413E-2</v>
       </c>
       <c r="V2">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L2)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L2),,)),,),0))</f>
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L2)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L2),,)),,),0))</f>
         <v>536</v>
       </c>
       <c r="W2">
@@ -624,14 +2684,14 @@
         <v>3.125E-2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E18" si="1">D3*A3</f>
+        <f t="shared" ref="E3:E18" si="2">D3*A3</f>
         <v>0.10312499999999999</v>
       </c>
       <c r="F3">
         <v>100</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G18" si="2">F3/((A3-E3)-1)</f>
+        <f t="shared" ref="G3:G18" si="3">F3/((A3-E3)-1)</f>
         <v>45.519203413940261</v>
       </c>
       <c r="H3">
@@ -642,51 +2702,51 @@
         <v>33000</v>
       </c>
       <c r="J3" s="2">
-        <f>I3*A3/E3-I3</f>
+        <f t="shared" si="1"/>
         <v>1023000</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K19" si="3">FLOOR(LOG(J3,10),1)-2</f>
+        <f t="shared" ref="K3:K19" si="4">FLOOR(LOG(J3,10),1)-2</f>
         <v>4</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" ref="L3:L18" si="4">J3/(10^K3)</f>
+        <f t="shared" ref="L3:L18" si="5">J3/(10^K3)</f>
         <v>102.3</v>
       </c>
       <c r="N3">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L3)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L3),,)),,),0))</f>
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L3)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L3),,)),,),0))</f>
         <v>100</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O19" si="5">N3*10^$K3</f>
+        <f t="shared" ref="O3:O19" si="6">N3*10^$K3</f>
         <v>1000000</v>
       </c>
       <c r="P3" s="1">
-        <f t="shared" ref="P3:P19" si="6">ABS($J3-O3)/O3</f>
+        <f t="shared" ref="P3:P19" si="7">ABS($J3-O3)/O3</f>
         <v>2.3E-2</v>
       </c>
       <c r="R3">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L3)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L3),,)),,),0))</f>
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L3)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L3),,)),,),0))</f>
         <v>100</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S19" si="7">R3*10^$K3</f>
+        <f t="shared" ref="S3:S19" si="8">R3*10^$K3</f>
         <v>1000000</v>
       </c>
       <c r="T3" s="5">
-        <f t="shared" ref="T3:T19" si="8">ABS($J3-S3)/S3</f>
+        <f t="shared" ref="T3:T19" si="9">ABS($J3-S3)/S3</f>
         <v>2.3E-2</v>
       </c>
       <c r="V3">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L3)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L3),,)),,),0))</f>
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L3)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L3),,)),,),0))</f>
         <v>100</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W19" si="9">V3*10^$K3</f>
+        <f t="shared" ref="W3:W19" si="10">V3*10^$K3</f>
         <v>1000000</v>
       </c>
       <c r="X3" s="1">
-        <f t="shared" ref="X3:X19" si="10">ABS($J3-W3)/W3</f>
+        <f t="shared" ref="X3:X19" si="11">ABS($J3-W3)/W3</f>
         <v>2.3E-2</v>
       </c>
     </row>
@@ -706,69 +2766,69 @@
         <v>9.375E-2</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.30937499999999996</v>
       </c>
       <c r="F4">
         <v>100</v>
       </c>
       <c r="G4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50.235478806907388</v>
       </c>
       <c r="H4">
         <v>150</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I19" si="11">I3</f>
+        <f t="shared" ref="I4:I19" si="12">I3</f>
         <v>33000</v>
       </c>
       <c r="J4" s="2">
-        <f>I4*A4/E4-I4</f>
+        <f t="shared" si="1"/>
         <v>319000.00000000006</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>319.00000000000006</v>
       </c>
       <c r="N4">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L4)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L4),,)),,),0))</f>
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L4)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L4),,)),,),0))</f>
         <v>330</v>
       </c>
       <c r="O4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>330000</v>
       </c>
       <c r="P4" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.3333333333333159E-2</v>
       </c>
       <c r="R4">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L4)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L4),,)),,),0))</f>
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L4)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L4),,)),,),0))</f>
         <v>330</v>
       </c>
       <c r="S4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>330000</v>
       </c>
       <c r="T4" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.3333333333333159E-2</v>
       </c>
       <c r="V4">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L4)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L4),,)),,),0))</f>
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L4)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L4),,)),,),0))</f>
         <v>316</v>
       </c>
       <c r="W4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>316000</v>
       </c>
       <c r="X4" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.4936708860761335E-3</v>
       </c>
     </row>
@@ -777,7 +2837,7 @@
         <v>3.3</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B18" si="12">B4+1</f>
+        <f t="shared" ref="B5:B18" si="13">B4+1</f>
         <v>2.5</v>
       </c>
       <c r="C5">
@@ -788,69 +2848,69 @@
         <v>0.15625</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.515625</v>
       </c>
       <c r="F5">
         <v>100</v>
       </c>
       <c r="G5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56.042031523642734</v>
       </c>
       <c r="H5">
         <v>180</v>
       </c>
       <c r="I5">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>178200</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="5"/>
+        <v>178.2</v>
+      </c>
+      <c r="N5">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L5)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L5),,)),,),0))</f>
+        <v>180</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="6"/>
+        <v>180000</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="7"/>
+        <v>0.01</v>
+      </c>
+      <c r="R5">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L5)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L5),,)),,),0))</f>
+        <v>180</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="8"/>
+        <v>180000</v>
+      </c>
+      <c r="T5" s="5">
+        <f t="shared" si="9"/>
+        <v>0.01</v>
+      </c>
+      <c r="V5">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L5)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L5),,)),,),0))</f>
+        <v>178</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="10"/>
+        <v>178000</v>
+      </c>
+      <c r="X5" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J5" s="2">
-        <f>I5*A5/E5-I5</f>
-        <v>178200</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="L5" s="3">
-        <f t="shared" si="4"/>
-        <v>178.2</v>
-      </c>
-      <c r="N5">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L5)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L5),,)),,),0))</f>
-        <v>180</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="5"/>
-        <v>180000</v>
-      </c>
-      <c r="P5" s="1">
-        <f t="shared" si="6"/>
-        <v>0.01</v>
-      </c>
-      <c r="R5">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L5)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L5),,)),,),0))</f>
-        <v>180</v>
-      </c>
-      <c r="S5">
-        <f t="shared" si="7"/>
-        <v>180000</v>
-      </c>
-      <c r="T5" s="5">
-        <f t="shared" si="8"/>
-        <v>0.01</v>
-      </c>
-      <c r="V5">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L5)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L5),,)),,),0))</f>
-        <v>178</v>
-      </c>
-      <c r="W5">
-        <f t="shared" si="9"/>
-        <v>178000</v>
-      </c>
-      <c r="X5" s="1">
-        <f t="shared" si="10"/>
         <v>1.1235955056179776E-3</v>
       </c>
     </row>
@@ -859,7 +2919,7 @@
         <v>3.3</v>
       </c>
       <c r="B6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.5</v>
       </c>
       <c r="C6">
@@ -870,69 +2930,69 @@
         <v>0.21875</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.72187499999999993</v>
       </c>
       <c r="F6">
         <v>100</v>
       </c>
       <c r="G6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>63.366336633663366</v>
       </c>
       <c r="H6">
         <v>220</v>
       </c>
       <c r="I6">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="1"/>
+        <v>117857.14285714287</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" si="5"/>
+        <v>117.85714285714288</v>
+      </c>
+      <c r="N6">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L6)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L6),,)),,),0))</f>
+        <v>120</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="6"/>
+        <v>120000</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="7"/>
+        <v>1.7857142857142752E-2</v>
+      </c>
+      <c r="R6">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L6)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L6),,)),,),0))</f>
+        <v>120</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="8"/>
+        <v>120000</v>
+      </c>
+      <c r="T6" s="5">
+        <f t="shared" si="9"/>
+        <v>1.7857142857142752E-2</v>
+      </c>
+      <c r="V6">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L6)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L6),,)),,),0))</f>
+        <v>115</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="10"/>
+        <v>115000</v>
+      </c>
+      <c r="X6" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J6" s="2">
-        <f>I6*A6/E6-I6</f>
-        <v>117857.14285714287</v>
-      </c>
-      <c r="K6" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="L6" s="3">
-        <f t="shared" si="4"/>
-        <v>117.85714285714288</v>
-      </c>
-      <c r="N6">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L6)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L6),,)),,),0))</f>
-        <v>120</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="5"/>
-        <v>120000</v>
-      </c>
-      <c r="P6" s="1">
-        <f t="shared" si="6"/>
-        <v>1.7857142857142752E-2</v>
-      </c>
-      <c r="R6">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L6)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L6),,)),,),0))</f>
-        <v>120</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="7"/>
-        <v>120000</v>
-      </c>
-      <c r="T6" s="5">
-        <f t="shared" si="8"/>
-        <v>1.7857142857142752E-2</v>
-      </c>
-      <c r="V6">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L6)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L6),,)),,),0))</f>
-        <v>115</v>
-      </c>
-      <c r="W6">
-        <f t="shared" si="9"/>
-        <v>115000</v>
-      </c>
-      <c r="X6" s="1">
-        <f t="shared" si="10"/>
         <v>2.4844720496894519E-2</v>
       </c>
     </row>
@@ -941,7 +3001,7 @@
         <v>3.3</v>
       </c>
       <c r="B7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.5</v>
       </c>
       <c r="C7">
@@ -952,69 +3012,69 @@
         <v>0.28125</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.92812499999999998</v>
       </c>
       <c r="F7">
         <v>100</v>
       </c>
       <c r="G7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>72.892938496583156</v>
       </c>
       <c r="H7">
         <v>270</v>
       </c>
       <c r="I7">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="1"/>
+        <v>84333.333333333343</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="5"/>
+        <v>843.33333333333348</v>
+      </c>
+      <c r="N7">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L7)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L7),,)),,),0))</f>
+        <v>820</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="6"/>
+        <v>82000</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="7"/>
+        <v>2.8455284552845645E-2</v>
+      </c>
+      <c r="R7">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L7)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L7),,)),,),0))</f>
+        <v>820</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="8"/>
+        <v>82000</v>
+      </c>
+      <c r="T7" s="5">
+        <f t="shared" si="9"/>
+        <v>2.8455284552845645E-2</v>
+      </c>
+      <c r="V7">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L7)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L7),,)),,),0))</f>
+        <v>825</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="10"/>
+        <v>82500</v>
+      </c>
+      <c r="X7" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J7" s="2">
-        <f>I7*A7/E7-I7</f>
-        <v>84333.333333333343</v>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L7" s="3">
-        <f t="shared" si="4"/>
-        <v>843.33333333333348</v>
-      </c>
-      <c r="N7">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L7)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L7),,)),,),0))</f>
-        <v>820</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="5"/>
-        <v>82000</v>
-      </c>
-      <c r="P7" s="1">
-        <f t="shared" si="6"/>
-        <v>2.8455284552845645E-2</v>
-      </c>
-      <c r="R7">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L7)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L7),,)),,),0))</f>
-        <v>820</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="7"/>
-        <v>82000</v>
-      </c>
-      <c r="T7" s="5">
-        <f t="shared" si="8"/>
-        <v>2.8455284552845645E-2</v>
-      </c>
-      <c r="V7">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L7)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L7),,)),,),0))</f>
-        <v>825</v>
-      </c>
-      <c r="W7">
-        <f t="shared" si="9"/>
-        <v>82500</v>
-      </c>
-      <c r="X7" s="1">
-        <f t="shared" si="10"/>
         <v>2.2222222222222341E-2</v>
       </c>
     </row>
@@ -1023,7 +3083,7 @@
         <v>3.3</v>
       </c>
       <c r="B8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.5</v>
       </c>
       <c r="C8">
@@ -1034,69 +3094,69 @@
         <v>0.34375</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1343749999999999</v>
       </c>
       <c r="F8">
         <v>100</v>
       </c>
       <c r="G8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85.79088471849866</v>
       </c>
       <c r="H8">
         <v>330</v>
       </c>
       <c r="I8">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="1"/>
+        <v>63000.000000000015</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="5"/>
+        <v>630.00000000000011</v>
+      </c>
+      <c r="N8">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L8)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L8),,)),,),0))</f>
+        <v>680</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="6"/>
+        <v>68000</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="7"/>
+        <v>7.3529411764705663E-2</v>
+      </c>
+      <c r="R8">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L8)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L8),,)),,),0))</f>
+        <v>620</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="8"/>
+        <v>62000</v>
+      </c>
+      <c r="T8" s="5">
+        <f t="shared" si="9"/>
+        <v>1.6129032258064752E-2</v>
+      </c>
+      <c r="V8">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L8)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L8),,)),,),0))</f>
+        <v>619</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="10"/>
+        <v>61900</v>
+      </c>
+      <c r="X8" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J8" s="2">
-        <f>I8*A8/E8-I8</f>
-        <v>63000.000000000015</v>
-      </c>
-      <c r="K8" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L8" s="3">
-        <f t="shared" si="4"/>
-        <v>630.00000000000011</v>
-      </c>
-      <c r="N8">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L8)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L8),,)),,),0))</f>
-        <v>680</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="5"/>
-        <v>68000</v>
-      </c>
-      <c r="P8" s="1">
-        <f t="shared" si="6"/>
-        <v>7.3529411764705663E-2</v>
-      </c>
-      <c r="R8">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L8)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L8),,)),,),0))</f>
-        <v>620</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="7"/>
-        <v>62000</v>
-      </c>
-      <c r="T8" s="5">
-        <f t="shared" si="8"/>
-        <v>1.6129032258064752E-2</v>
-      </c>
-      <c r="V8">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L8)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L8),,)),,),0))</f>
-        <v>619</v>
-      </c>
-      <c r="W8">
-        <f t="shared" si="9"/>
-        <v>61900</v>
-      </c>
-      <c r="X8" s="1">
-        <f t="shared" si="10"/>
         <v>1.7770597738287795E-2</v>
       </c>
     </row>
@@ -1105,7 +3165,7 @@
         <v>3.3</v>
       </c>
       <c r="B9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6.5</v>
       </c>
       <c r="C9">
@@ -1116,69 +3176,69 @@
         <v>0.40625</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.340625</v>
       </c>
       <c r="F9">
         <v>100</v>
       </c>
       <c r="G9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>104.23452768729643</v>
       </c>
       <c r="H9">
         <v>390</v>
       </c>
       <c r="I9">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>48230.769230769234</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="5"/>
+        <v>482.30769230769232</v>
+      </c>
+      <c r="N9">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L9)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L9),,)),,),0))</f>
+        <v>470</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="6"/>
+        <v>47000</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="7"/>
+        <v>2.618657937806881E-2</v>
+      </c>
+      <c r="R9">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L9)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L9),,)),,),0))</f>
+        <v>470</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="8"/>
+        <v>47000</v>
+      </c>
+      <c r="T9" s="5">
+        <f t="shared" si="9"/>
+        <v>2.618657937806881E-2</v>
+      </c>
+      <c r="V9">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L9)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L9),,)),,),0))</f>
+        <v>487</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="10"/>
+        <v>48700</v>
+      </c>
+      <c r="X9" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J9" s="2">
-        <f>I9*A9/E9-I9</f>
-        <v>48230.769230769234</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L9" s="3">
-        <f t="shared" si="4"/>
-        <v>482.30769230769232</v>
-      </c>
-      <c r="N9">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L9)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L9),,)),,),0))</f>
-        <v>470</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="5"/>
-        <v>47000</v>
-      </c>
-      <c r="P9" s="1">
-        <f t="shared" si="6"/>
-        <v>2.618657937806881E-2</v>
-      </c>
-      <c r="R9">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L9)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L9),,)),,),0))</f>
-        <v>470</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="7"/>
-        <v>47000</v>
-      </c>
-      <c r="T9" s="5">
-        <f t="shared" si="8"/>
-        <v>2.618657937806881E-2</v>
-      </c>
-      <c r="V9">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L9)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L9),,)),,),0))</f>
-        <v>487</v>
-      </c>
-      <c r="W9">
-        <f t="shared" si="9"/>
-        <v>48700</v>
-      </c>
-      <c r="X9" s="1">
-        <f t="shared" si="10"/>
         <v>9.6351287316379028E-3</v>
       </c>
     </row>
@@ -1187,7 +3247,7 @@
         <v>3.3</v>
       </c>
       <c r="B10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7.5</v>
       </c>
       <c r="C10">
@@ -1198,69 +3258,69 @@
         <v>0.46875</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.546875</v>
       </c>
       <c r="F10">
         <v>100</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>132.78008298755191</v>
       </c>
       <c r="H10">
         <v>470</v>
       </c>
       <c r="I10">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>37400</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="5"/>
+        <v>374</v>
+      </c>
+      <c r="N10">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L10)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L10),,)),,),0))</f>
+        <v>390</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>39000</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" si="7"/>
+        <v>4.1025641025641026E-2</v>
+      </c>
+      <c r="R10">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L10)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L10),,)),,),0))</f>
+        <v>360</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="8"/>
+        <v>36000</v>
+      </c>
+      <c r="T10" s="5">
+        <f t="shared" si="9"/>
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="V10">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L10)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L10),,)),,),0))</f>
+        <v>365</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="10"/>
+        <v>36500</v>
+      </c>
+      <c r="X10" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J10" s="2">
-        <f>I10*A10/E10-I10</f>
-        <v>37400</v>
-      </c>
-      <c r="K10" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L10" s="3">
-        <f t="shared" si="4"/>
-        <v>374</v>
-      </c>
-      <c r="N10">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L10)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L10),,)),,),0))</f>
-        <v>390</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="5"/>
-        <v>39000</v>
-      </c>
-      <c r="P10" s="1">
-        <f t="shared" si="6"/>
-        <v>4.1025641025641026E-2</v>
-      </c>
-      <c r="R10">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L10)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L10),,)),,),0))</f>
-        <v>360</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="7"/>
-        <v>36000</v>
-      </c>
-      <c r="T10" s="5">
-        <f t="shared" si="8"/>
-        <v>3.888888888888889E-2</v>
-      </c>
-      <c r="V10">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L10)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L10),,)),,),0))</f>
-        <v>365</v>
-      </c>
-      <c r="W10">
-        <f t="shared" si="9"/>
-        <v>36500</v>
-      </c>
-      <c r="X10" s="1">
-        <f t="shared" si="10"/>
         <v>2.4657534246575342E-2</v>
       </c>
     </row>
@@ -1269,7 +3329,7 @@
         <v>3.3</v>
       </c>
       <c r="B11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8.5</v>
       </c>
       <c r="C11">
@@ -1280,69 +3340,69 @@
         <v>0.53125</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7531249999999998</v>
       </c>
       <c r="F11">
         <v>100</v>
       </c>
       <c r="G11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>182.85714285714286</v>
       </c>
       <c r="H11">
         <v>560</v>
       </c>
       <c r="I11">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>29117.647058823539</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="5"/>
+        <v>291.17647058823536</v>
+      </c>
+      <c r="N11">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L11)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L11),,)),,),0))</f>
+        <v>270</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="6"/>
+        <v>27000</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="7"/>
+        <v>7.8431372549019954E-2</v>
+      </c>
+      <c r="R11">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L11)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L11),,)),,),0))</f>
+        <v>300</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="8"/>
+        <v>30000</v>
+      </c>
+      <c r="T11" s="5">
+        <f t="shared" si="9"/>
+        <v>2.941176470588204E-2</v>
+      </c>
+      <c r="V11">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L11)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L11),,)),,),0))</f>
+        <v>287</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="10"/>
+        <v>28700</v>
+      </c>
+      <c r="X11" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J11" s="2">
-        <f>I11*A11/E11-I11</f>
-        <v>29117.647058823539</v>
-      </c>
-      <c r="K11" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L11" s="3">
-        <f t="shared" si="4"/>
-        <v>291.17647058823536</v>
-      </c>
-      <c r="N11">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L11)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L11),,)),,),0))</f>
-        <v>270</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="5"/>
-        <v>27000</v>
-      </c>
-      <c r="P11" s="1">
-        <f t="shared" si="6"/>
-        <v>7.8431372549019954E-2</v>
-      </c>
-      <c r="R11">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L11)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L11),,)),,),0))</f>
-        <v>300</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="7"/>
-        <v>30000</v>
-      </c>
-      <c r="T11" s="5">
-        <f t="shared" si="8"/>
-        <v>2.941176470588204E-2</v>
-      </c>
-      <c r="V11">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L11)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L11),,)),,),0))</f>
-        <v>287</v>
-      </c>
-      <c r="W11">
-        <f t="shared" si="9"/>
-        <v>28700</v>
-      </c>
-      <c r="X11" s="1">
-        <f t="shared" si="10"/>
         <v>1.45521623283463E-2</v>
       </c>
     </row>
@@ -1351,7 +3411,7 @@
         <v>3.3</v>
       </c>
       <c r="B12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>9.5</v>
       </c>
       <c r="C12">
@@ -1362,69 +3422,69 @@
         <v>0.59375</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9593749999999999</v>
       </c>
       <c r="F12">
         <v>100</v>
       </c>
       <c r="G12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>293.57798165137621</v>
       </c>
       <c r="H12">
         <v>680</v>
       </c>
       <c r="I12">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>22578.947368421053</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="5"/>
+        <v>225.78947368421052</v>
+      </c>
+      <c r="N12">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L12)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L12),,)),,),0))</f>
+        <v>220</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="6"/>
+        <v>22000</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="7"/>
+        <v>2.6315789473684244E-2</v>
+      </c>
+      <c r="R12">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L12)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L12),,)),,),0))</f>
+        <v>220</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="8"/>
+        <v>22000</v>
+      </c>
+      <c r="T12" s="5">
+        <f t="shared" si="9"/>
+        <v>2.6315789473684244E-2</v>
+      </c>
+      <c r="V12">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L12)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L12),,)),,),0))</f>
+        <v>226</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="10"/>
+        <v>22600</v>
+      </c>
+      <c r="X12" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J12" s="2">
-        <f>I12*A12/E12-I12</f>
-        <v>22578.947368421053</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L12" s="3">
-        <f t="shared" si="4"/>
-        <v>225.78947368421052</v>
-      </c>
-      <c r="N12">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L12)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L12),,)),,),0))</f>
-        <v>220</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="5"/>
-        <v>22000</v>
-      </c>
-      <c r="P12" s="1">
-        <f t="shared" si="6"/>
-        <v>2.6315789473684244E-2</v>
-      </c>
-      <c r="R12">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L12)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L12),,)),,),0))</f>
-        <v>220</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="7"/>
-        <v>22000</v>
-      </c>
-      <c r="T12" s="5">
-        <f t="shared" si="8"/>
-        <v>2.6315789473684244E-2</v>
-      </c>
-      <c r="V12">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L12)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L12),,)),,),0))</f>
-        <v>226</v>
-      </c>
-      <c r="W12">
-        <f t="shared" si="9"/>
-        <v>22600</v>
-      </c>
-      <c r="X12" s="1">
-        <f t="shared" si="10"/>
         <v>9.3153237074984966E-4</v>
       </c>
     </row>
@@ -1433,7 +3493,7 @@
         <v>3.3</v>
       </c>
       <c r="B13">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>10.5</v>
       </c>
       <c r="C13">
@@ -1444,69 +3504,69 @@
         <v>0.65625</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.1656249999999999</v>
       </c>
       <c r="F13">
         <v>100</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>744.18604651162843</v>
       </c>
       <c r="H13">
         <v>820</v>
       </c>
       <c r="I13">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>17285.71428571429</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="5"/>
+        <v>172.85714285714289</v>
+      </c>
+      <c r="N13">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L13)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L13),,)),,),0))</f>
+        <v>180</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="6"/>
+        <v>18000</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="7"/>
+        <v>3.9682539682539451E-2</v>
+      </c>
+      <c r="R13">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L13)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L13),,)),,),0))</f>
+        <v>180</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="8"/>
+        <v>18000</v>
+      </c>
+      <c r="T13" s="5">
+        <f t="shared" si="9"/>
+        <v>3.9682539682539451E-2</v>
+      </c>
+      <c r="V13">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L13)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L13),,)),,),0))</f>
+        <v>169</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="10"/>
+        <v>16900</v>
+      </c>
+      <c r="X13" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J13" s="2">
-        <f>I13*A13/E13-I13</f>
-        <v>17285.71428571429</v>
-      </c>
-      <c r="K13" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L13" s="3">
-        <f t="shared" si="4"/>
-        <v>172.85714285714289</v>
-      </c>
-      <c r="N13">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L13)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L13),,)),,),0))</f>
-        <v>180</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="5"/>
-        <v>18000</v>
-      </c>
-      <c r="P13" s="1">
-        <f t="shared" si="6"/>
-        <v>3.9682539682539451E-2</v>
-      </c>
-      <c r="R13">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L13)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L13),,)),,),0))</f>
-        <v>180</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="7"/>
-        <v>18000</v>
-      </c>
-      <c r="T13" s="5">
-        <f t="shared" si="8"/>
-        <v>3.9682539682539451E-2</v>
-      </c>
-      <c r="V13">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L13)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L13),,)),,),0))</f>
-        <v>169</v>
-      </c>
-      <c r="W13">
-        <f t="shared" si="9"/>
-        <v>16900</v>
-      </c>
-      <c r="X13" s="1">
-        <f t="shared" si="10"/>
         <v>2.2823330515638455E-2</v>
       </c>
     </row>
@@ -1515,7 +3575,7 @@
         <v>3.3</v>
       </c>
       <c r="B14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>11.5</v>
       </c>
       <c r="C14">
@@ -1526,66 +3586,66 @@
         <v>0.71875</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3718749999999997</v>
       </c>
       <c r="F14">
         <v>100</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1391.3043478260886</v>
       </c>
       <c r="I14">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>12913.043478260872</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="5"/>
+        <v>129.13043478260872</v>
+      </c>
+      <c r="N14">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L14)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L14),,)),,),0))</f>
+        <v>120</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="6"/>
+        <v>12000</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="7"/>
+        <v>7.6086956521739316E-2</v>
+      </c>
+      <c r="R14">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L14)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L14),,)),,),0))</f>
+        <v>130</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="8"/>
+        <v>13000</v>
+      </c>
+      <c r="T14" s="5">
+        <f t="shared" si="9"/>
+        <v>6.688963210702171E-3</v>
+      </c>
+      <c r="V14">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L14)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L14),,)),,),0))</f>
+        <v>127</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="10"/>
+        <v>12700</v>
+      </c>
+      <c r="X14" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J14" s="2">
-        <f>I14*A14/E14-I14</f>
-        <v>12913.043478260872</v>
-      </c>
-      <c r="K14" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L14" s="3">
-        <f t="shared" si="4"/>
-        <v>129.13043478260872</v>
-      </c>
-      <c r="N14">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L14)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L14),,)),,),0))</f>
-        <v>120</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="5"/>
-        <v>12000</v>
-      </c>
-      <c r="P14" s="1">
-        <f t="shared" si="6"/>
-        <v>7.6086956521739316E-2</v>
-      </c>
-      <c r="R14">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L14)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L14),,)),,),0))</f>
-        <v>130</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="7"/>
-        <v>13000</v>
-      </c>
-      <c r="T14" s="5">
-        <f t="shared" si="8"/>
-        <v>6.688963210702171E-3</v>
-      </c>
-      <c r="V14">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L14)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L14),,)),,),0))</f>
-        <v>127</v>
-      </c>
-      <c r="W14">
-        <f t="shared" si="9"/>
-        <v>12700</v>
-      </c>
-      <c r="X14" s="1">
-        <f t="shared" si="10"/>
         <v>1.6775077028415099E-2</v>
       </c>
     </row>
@@ -1594,7 +3654,7 @@
         <v>3.3</v>
       </c>
       <c r="B15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>12.5</v>
       </c>
       <c r="C15">
@@ -1605,66 +3665,66 @@
         <v>0.78125</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.578125</v>
       </c>
       <c r="F15">
         <v>100</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-359.55056179775261</v>
       </c>
       <c r="I15">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="1"/>
+        <v>9240</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="5"/>
+        <v>924</v>
+      </c>
+      <c r="N15">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L15)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L15),,)),,),0))</f>
+        <v>820</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="6"/>
+        <v>8200</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" si="7"/>
+        <v>0.12682926829268293</v>
+      </c>
+      <c r="R15">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L15)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L15),,)),,),0))</f>
+        <v>910</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="8"/>
+        <v>9100</v>
+      </c>
+      <c r="T15" s="5">
+        <f t="shared" si="9"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="V15">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L15)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L15),,)),,),0))</f>
+        <v>909</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="10"/>
+        <v>9090</v>
+      </c>
+      <c r="X15" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J15" s="2">
-        <f>I15*A15/E15-I15</f>
-        <v>9240</v>
-      </c>
-      <c r="K15" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L15" s="3">
-        <f t="shared" si="4"/>
-        <v>924</v>
-      </c>
-      <c r="N15">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L15)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L15),,)),,),0))</f>
-        <v>820</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="5"/>
-        <v>8200</v>
-      </c>
-      <c r="P15" s="1">
-        <f t="shared" si="6"/>
-        <v>0.12682926829268293</v>
-      </c>
-      <c r="R15">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L15)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L15),,)),,),0))</f>
-        <v>910</v>
-      </c>
-      <c r="S15">
-        <f t="shared" si="7"/>
-        <v>9100</v>
-      </c>
-      <c r="T15" s="5">
-        <f t="shared" si="8"/>
-        <v>1.5384615384615385E-2</v>
-      </c>
-      <c r="V15">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L15)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L15),,)),,),0))</f>
-        <v>909</v>
-      </c>
-      <c r="W15">
-        <f t="shared" si="9"/>
-        <v>9090</v>
-      </c>
-      <c r="X15" s="1">
-        <f t="shared" si="10"/>
         <v>1.65016501650165E-2</v>
       </c>
     </row>
@@ -1673,7 +3733,7 @@
         <v>3.3</v>
       </c>
       <c r="B16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>13.5</v>
       </c>
       <c r="C16">
@@ -1684,66 +3744,66 @@
         <v>0.84375</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.7843749999999998</v>
       </c>
       <c r="F16">
         <v>100</v>
       </c>
       <c r="G16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-206.45161290322579</v>
       </c>
       <c r="I16">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="1"/>
+        <v>6111.1111111111168</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="5"/>
+        <v>611.11111111111165</v>
+      </c>
+      <c r="N16">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L16)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L16),,)),,),0))</f>
+        <v>560</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="6"/>
+        <v>5600</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" si="7"/>
+        <v>9.1269841269842278E-2</v>
+      </c>
+      <c r="R16">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L16)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L16),,)),,),0))</f>
+        <v>620</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="8"/>
+        <v>6200</v>
+      </c>
+      <c r="T16" s="5">
+        <f t="shared" si="9"/>
+        <v>1.4336917562723102E-2</v>
+      </c>
+      <c r="V16">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L16)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L16),,)),,),0))</f>
+        <v>619</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="10"/>
+        <v>6190</v>
+      </c>
+      <c r="X16" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J16" s="2">
-        <f>I16*A16/E16-I16</f>
-        <v>6111.1111111111168</v>
-      </c>
-      <c r="K16" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L16" s="3">
-        <f t="shared" si="4"/>
-        <v>611.11111111111165</v>
-      </c>
-      <c r="N16">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L16)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L16),,)),,),0))</f>
-        <v>560</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="5"/>
-        <v>5600</v>
-      </c>
-      <c r="P16" s="1">
-        <f t="shared" si="6"/>
-        <v>9.1269841269842278E-2</v>
-      </c>
-      <c r="R16">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L16)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L16),,)),,),0))</f>
-        <v>620</v>
-      </c>
-      <c r="S16">
-        <f t="shared" si="7"/>
-        <v>6200</v>
-      </c>
-      <c r="T16" s="5">
-        <f t="shared" si="8"/>
-        <v>1.4336917562723102E-2</v>
-      </c>
-      <c r="V16">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L16)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L16),,)),,),0))</f>
-        <v>619</v>
-      </c>
-      <c r="W16">
-        <f t="shared" si="9"/>
-        <v>6190</v>
-      </c>
-      <c r="X16" s="1">
-        <f t="shared" si="10"/>
         <v>1.2744570095134609E-2</v>
       </c>
     </row>
@@ -1752,7 +3812,7 @@
         <v>3.3</v>
       </c>
       <c r="B17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>14.5</v>
       </c>
       <c r="C17">
@@ -1763,66 +3823,66 @@
         <v>0.90625</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9906249999999996</v>
       </c>
       <c r="F17">
         <v>100</v>
       </c>
       <c r="G17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-144.79638009049776</v>
       </c>
       <c r="I17">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="1"/>
+        <v>3413.7931034482826</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" si="5"/>
+        <v>341.37931034482824</v>
+      </c>
+      <c r="N17">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L17)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L17),,)),,),0))</f>
+        <v>330</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="6"/>
+        <v>3300</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" si="7"/>
+        <v>3.4482758620691709E-2</v>
+      </c>
+      <c r="R17">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L17)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L17),,)),,),0))</f>
+        <v>330</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="8"/>
+        <v>3300</v>
+      </c>
+      <c r="T17" s="5">
+        <f t="shared" si="9"/>
+        <v>3.4482758620691709E-2</v>
+      </c>
+      <c r="V17">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L17)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L17),,)),,),0))</f>
+        <v>348</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="10"/>
+        <v>3480</v>
+      </c>
+      <c r="X17" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J17" s="2">
-        <f>I17*A17/E17-I17</f>
-        <v>3413.7931034482826</v>
-      </c>
-      <c r="K17" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L17" s="3">
-        <f t="shared" si="4"/>
-        <v>341.37931034482824</v>
-      </c>
-      <c r="N17">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L17)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L17),,)),,),0))</f>
-        <v>330</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="5"/>
-        <v>3300</v>
-      </c>
-      <c r="P17" s="1">
-        <f t="shared" si="6"/>
-        <v>3.4482758620691709E-2</v>
-      </c>
-      <c r="R17">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L17)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L17),,)),,),0))</f>
-        <v>330</v>
-      </c>
-      <c r="S17">
-        <f t="shared" si="7"/>
-        <v>3300</v>
-      </c>
-      <c r="T17" s="5">
-        <f t="shared" si="8"/>
-        <v>3.4482758620691709E-2</v>
-      </c>
-      <c r="V17">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L17)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L17),,)),,),0))</f>
-        <v>348</v>
-      </c>
-      <c r="W17">
-        <f t="shared" si="9"/>
-        <v>3480</v>
-      </c>
-      <c r="X17" s="1">
-        <f t="shared" si="10"/>
         <v>1.9024970273482E-2</v>
       </c>
     </row>
@@ -1831,7 +3891,7 @@
         <v>3.3</v>
       </c>
       <c r="B18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>15.5</v>
       </c>
       <c r="C18">
@@ -1842,66 +3902,66 @@
         <v>0.96875</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.1968749999999999</v>
       </c>
       <c r="F18">
         <v>100</v>
       </c>
       <c r="G18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-111.49825783972125</v>
       </c>
       <c r="I18">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="1"/>
+        <v>1064.5161290322576</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" si="5"/>
+        <v>106.45161290322577</v>
+      </c>
+      <c r="N18">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L18)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L18),,)),,),0))</f>
+        <v>100</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="6"/>
+        <v>1000</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="7"/>
+        <v>6.4516129032257591E-2</v>
+      </c>
+      <c r="R18">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L18)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L18),,)),,),0))</f>
+        <v>110</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="8"/>
+        <v>1100</v>
+      </c>
+      <c r="T18" s="5">
+        <f t="shared" si="9"/>
+        <v>3.2258064516129462E-2</v>
+      </c>
+      <c r="V18">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L18)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L18),,)),,),0))</f>
+        <v>105</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="10"/>
+        <v>1050</v>
+      </c>
+      <c r="X18" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J18" s="2">
-        <f>I18*A18/E18-I18</f>
-        <v>1064.5161290322576</v>
-      </c>
-      <c r="K18" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L18" s="3">
-        <f t="shared" si="4"/>
-        <v>106.45161290322577</v>
-      </c>
-      <c r="N18">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L18)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L18),,)),,),0))</f>
-        <v>100</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="5"/>
-        <v>1000</v>
-      </c>
-      <c r="P18" s="1">
-        <f t="shared" si="6"/>
-        <v>6.4516129032257591E-2</v>
-      </c>
-      <c r="R18">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L18)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L18),,)),,),0))</f>
-        <v>110</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="7"/>
-        <v>1100</v>
-      </c>
-      <c r="T18" s="5">
-        <f t="shared" si="8"/>
-        <v>3.2258064516129462E-2</v>
-      </c>
-      <c r="V18">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L18)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L18),,)),,),0))</f>
-        <v>105</v>
-      </c>
-      <c r="W18">
-        <f t="shared" si="9"/>
-        <v>1050</v>
-      </c>
-      <c r="X18" s="1">
-        <f t="shared" si="10"/>
         <v>1.3824884792626281E-2</v>
       </c>
     </row>
@@ -1916,70 +3976,70 @@
         <v>16</v>
       </c>
       <c r="D19">
-        <f t="shared" ref="D19" si="13">B19/C19</f>
+        <f t="shared" ref="D19" si="14">B19/C19</f>
         <v>0.99937500000000001</v>
       </c>
       <c r="E19">
-        <f t="shared" ref="E19" si="14">D19*A19</f>
+        <f t="shared" ref="E19" si="15">D19*A19</f>
         <v>3.2979374999999997</v>
       </c>
       <c r="F19">
         <v>100</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19" si="15">F19/((A19-E19)-1)</f>
+        <f t="shared" ref="G19" si="16">F19/((A19-E19)-1)</f>
         <v>-100.20667626980648</v>
       </c>
       <c r="I19">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="1"/>
+        <v>20.637898686683911</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" ref="L19" si="17">J19/(10^K19)</f>
+        <v>206.37898686683911</v>
+      </c>
+      <c r="N19">
+        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L19)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-'100kDividers'!$L19),,)),,),0))</f>
+        <v>220</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+      <c r="P19" s="1">
+        <f t="shared" si="7"/>
+        <v>6.1913696059822214E-2</v>
+      </c>
+      <c r="R19">
+        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L19)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-'100kDividers'!$L19),,)),,),0))</f>
+        <v>200</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="T19" s="5">
+        <f t="shared" si="9"/>
+        <v>3.1894934334195567E-2</v>
+      </c>
+      <c r="V19">
+        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L19)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-'100kDividers'!$L19),,)),,),0))</f>
+        <v>205</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="10"/>
+        <v>20.5</v>
+      </c>
+      <c r="X19" s="1">
         <f t="shared" si="11"/>
-        <v>33000</v>
-      </c>
-      <c r="J19" s="2">
-        <f>I19*A19/E19-I19</f>
-        <v>20.637898686683911</v>
-      </c>
-      <c r="K19" s="3">
-        <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="L19" s="3">
-        <f t="shared" ref="L19" si="16">J19/(10^K19)</f>
-        <v>206.37898686683911</v>
-      </c>
-      <c r="N19">
-        <f>INDEX(Resistors!$B$2:$B$49,MATCH(TRUE,INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L19)=MIN(INDEX(ABS(Resistors!$B$2:$B$49-Dividers!$L19),,)),,),0))</f>
-        <v>220</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="5"/>
-        <v>22</v>
-      </c>
-      <c r="P19" s="1">
-        <f t="shared" si="6"/>
-        <v>6.1913696059822214E-2</v>
-      </c>
-      <c r="R19">
-        <f>INDEX(Resistors!$C$2:$C$49,MATCH(TRUE,INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L19)=MIN(INDEX(ABS(Resistors!$C$2:$C$49-Dividers!$L19),,)),,),0))</f>
-        <v>200</v>
-      </c>
-      <c r="S19">
-        <f t="shared" si="7"/>
-        <v>20</v>
-      </c>
-      <c r="T19" s="5">
-        <f t="shared" si="8"/>
-        <v>3.1894934334195567E-2</v>
-      </c>
-      <c r="V19">
-        <f>INDEX(Resistors!$D$2:$D$49,MATCH(TRUE,INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L19)=MIN(INDEX(ABS(Resistors!$D$2:$D$49-Dividers!$L19),,)),,),0))</f>
-        <v>205</v>
-      </c>
-      <c r="W19">
-        <f t="shared" si="9"/>
-        <v>20.5</v>
-      </c>
-      <c r="X19" s="1">
-        <f t="shared" si="10"/>
         <v>6.7267652040932371E-3</v>
       </c>
     </row>
@@ -2155,11 +4215,11 @@
         <v>3.96825396825395E-2</v>
       </c>
       <c r="Q30" s="3">
-        <f t="shared" ref="Q30:Q44" si="17">Q29+1</f>
+        <f t="shared" ref="Q30:Q44" si="18">Q29+1</f>
         <v>3</v>
       </c>
       <c r="R30">
-        <f t="shared" ref="R30:R43" si="18">R29+2</f>
+        <f t="shared" ref="R30:R43" si="19">R29+2</f>
         <v>4.5</v>
       </c>
       <c r="S30">
@@ -2183,11 +4243,11 @@
         <v>9.5238095238095316E-2</v>
       </c>
       <c r="Q31" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="R31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.5</v>
       </c>
       <c r="S31">
@@ -2211,11 +4271,11 @@
         <v>5.7500000000000002E-2</v>
       </c>
       <c r="Q32" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="R32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8.5</v>
       </c>
       <c r="S32">
@@ -2239,11 +4299,11 @@
         <v>4.5925925925925939E-2</v>
       </c>
       <c r="Q33" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="R33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>10.5</v>
       </c>
       <c r="S33">
@@ -2270,11 +4330,11 @@
         <v>9.2138630600169025E-2</v>
       </c>
       <c r="Q34" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7</v>
       </c>
       <c r="R34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>12.5</v>
       </c>
       <c r="S34">
@@ -2301,11 +4361,11 @@
         <v>8</v>
       </c>
       <c r="Q35" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="R35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>14.5</v>
       </c>
       <c r="S35">
@@ -2320,11 +4380,11 @@
     </row>
     <row r="36" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q36" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="R36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>16.5</v>
       </c>
       <c r="S36">
@@ -2336,11 +4396,11 @@
     </row>
     <row r="37" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q37" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="R37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>18.5</v>
       </c>
       <c r="S37">
@@ -2355,11 +4415,11 @@
     </row>
     <row r="38" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q38" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="R38">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>20.5</v>
       </c>
       <c r="S38">
@@ -2377,11 +4437,11 @@
     </row>
     <row r="39" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q39" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="R39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>22.5</v>
       </c>
       <c r="S39">
@@ -2396,11 +4456,11 @@
     </row>
     <row r="40" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q40" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="R40">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>24.5</v>
       </c>
       <c r="S40">
@@ -2415,11 +4475,11 @@
     </row>
     <row r="41" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q41" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="R41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>26.5</v>
       </c>
       <c r="S41">
@@ -2437,11 +4497,11 @@
     </row>
     <row r="42" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q42" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="R42">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>28.5</v>
       </c>
       <c r="S42">
@@ -2462,11 +4522,11 @@
         <v>16</v>
       </c>
       <c r="Q43" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="R43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>30.5</v>
       </c>
       <c r="S43">
@@ -2484,7 +4544,7 @@
     </row>
     <row r="44" spans="9:25" x14ac:dyDescent="0.25">
       <c r="Q44" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>17</v>
       </c>
       <c r="R44">
@@ -2503,7 +4563,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>

</xml_diff>